<commit_message>
TP#21774: Adding SaveLabel column
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/2017/CA Exp Dom.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/2017/CA Exp Dom.xlsx
@@ -15,7 +15,7 @@
     <sheet name="CA Exp Dom" sheetId="43" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CA Exp Dom'!$A$2:$JM$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CA Exp Dom'!$A$2:$JN$2</definedName>
     <definedName name="_lu1" localSheetId="0">#REF!</definedName>
     <definedName name="_lu1">#REF!</definedName>
     <definedName name="_lu2" localSheetId="0">#REF!</definedName>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="183">
   <si>
     <t>CUSTOMER_REFERENCE</t>
   </si>
@@ -572,6 +572,9 @@
   </si>
   <si>
     <t>Revenue+Labels</t>
+  </si>
+  <si>
+    <t>SaveLabel</t>
   </si>
 </sst>
 </file>
@@ -683,12 +686,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -779,6 +776,11 @@
     <font>
       <b/>
       <sz val="16"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -1111,236 +1113,236 @@
   </borders>
   <cellStyleXfs count="363">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
@@ -1349,23 +1351,23 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
@@ -1381,10 +1383,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
@@ -1444,7 +1446,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1457,94 +1459,114 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="2" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="2" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="2" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="5" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="5" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1559,135 +1581,121 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="25" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="2" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="23" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="24" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="24" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="363">
@@ -2411,7 +2419,7 @@
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3:D12"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2484,16 +2492,16 @@
     <col min="151" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" s="18" customFormat="1" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="17"/>
-      <c r="C1" s="17" t="s">
+    <row r="1" spans="1:89" s="18" customFormat="1" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="77" t="s">
+        <v>182</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>37</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>49</v>
       </c>
       <c r="F1" s="20" t="s">
         <v>49</v>
@@ -2505,13 +2513,13 @@
         <v>49</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="J1" s="20" t="s">
         <v>111</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="L1" s="20" t="s">
         <v>95</v>
@@ -2520,7 +2528,7 @@
         <v>95</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>140</v>
+        <v>95</v>
       </c>
       <c r="O1" s="20" t="s">
         <v>140</v>
@@ -2535,7 +2543,7 @@
         <v>140</v>
       </c>
       <c r="S1" s="20" t="s">
-        <v>51</v>
+        <v>140</v>
       </c>
       <c r="T1" s="20" t="s">
         <v>51</v>
@@ -2544,7 +2552,7 @@
         <v>51</v>
       </c>
       <c r="V1" s="20" t="s">
-        <v>141</v>
+        <v>51</v>
       </c>
       <c r="W1" s="20" t="s">
         <v>141</v>
@@ -2558,32 +2566,32 @@
       <c r="Z1" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="AA1" s="16" t="s">
+      <c r="AA1" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB1" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AC1" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="AC1" s="16" t="s">
+      <c r="AD1" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="AD1" s="16" t="s">
+      <c r="AE1" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="AE1" s="20" t="s">
+      <c r="AF1" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="AF1" s="20" t="s">
+      <c r="AG1" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="AG1" s="17" t="s">
+      <c r="AH1" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="AH1" s="20" t="s">
+      <c r="AI1" s="20" t="s">
         <v>148</v>
-      </c>
-      <c r="AI1" s="20" t="s">
-        <v>147</v>
       </c>
       <c r="AJ1" s="20" t="s">
         <v>147</v>
@@ -2592,7 +2600,7 @@
         <v>147</v>
       </c>
       <c r="AL1" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AM1" s="20" t="s">
         <v>149</v>
@@ -2606,35 +2614,35 @@
       <c r="AP1" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="AQ1" s="22" t="s">
+      <c r="AQ1" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="AR1" s="22" t="s">
         <v>179</v>
-      </c>
-      <c r="AR1" s="22" t="s">
-        <v>166</v>
       </c>
       <c r="AS1" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="AT1" s="21" t="s">
+      <c r="AT1" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="AU1" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="AU1" s="20" t="s">
+      <c r="AV1" s="20" t="s">
         <v>49</v>
-      </c>
-      <c r="AV1" s="20" t="s">
-        <v>151</v>
       </c>
       <c r="AW1" s="20" t="s">
         <v>151</v>
       </c>
       <c r="AX1" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AY1" s="20" t="s">
         <v>152</v>
       </c>
       <c r="AZ1" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BA1" s="20" t="s">
         <v>153</v>
@@ -2646,61 +2654,61 @@
         <v>153</v>
       </c>
       <c r="BD1" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BE1" s="20" t="s">
         <v>154</v>
       </c>
       <c r="BF1" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="BG1" s="20" t="s">
         <v>155</v>
-      </c>
-      <c r="BG1" s="20" t="s">
-        <v>156</v>
       </c>
       <c r="BH1" s="20" t="s">
         <v>156</v>
       </c>
       <c r="BI1" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BJ1" s="20" t="s">
         <v>157</v>
       </c>
       <c r="BK1" s="20" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="BL1" s="20" t="s">
         <v>172</v>
       </c>
       <c r="BM1" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="BN1" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="BN1" s="20" t="s">
+      <c r="BO1" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="BO1" s="20" t="s">
+      <c r="BP1" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="BP1" s="20" t="s">
+      <c r="BQ1" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="BQ1" s="19" t="s">
+      <c r="BR1" s="19" t="s">
         <v>180</v>
-      </c>
-      <c r="BR1" s="19" t="s">
-        <v>158</v>
       </c>
       <c r="BS1" s="19" t="s">
         <v>158</v>
       </c>
       <c r="BT1" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BU1" s="19" t="s">
         <v>159</v>
       </c>
       <c r="BV1" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="BW1" s="19" t="s">
         <v>160</v>
@@ -2709,25 +2717,25 @@
         <v>160</v>
       </c>
       <c r="BY1" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="BZ1" s="19" t="s">
         <v>161</v>
       </c>
       <c r="CA1" s="19" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="CB1" s="19" t="s">
         <v>160</v>
       </c>
       <c r="CC1" s="19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="CD1" s="19" t="s">
         <v>162</v>
       </c>
       <c r="CE1" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="CF1" s="19" t="s">
         <v>163</v>
@@ -2738,360 +2746,366 @@
       <c r="CH1" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="CI1" s="20" t="s">
-        <v>164</v>
+      <c r="CI1" s="19" t="s">
+        <v>163</v>
       </c>
       <c r="CJ1" s="20" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="2" spans="1:88" s="9" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="CK1" s="20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:89" s="9" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="AB2" s="39" t="s">
+      <c r="AC2" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="AC2" s="39" t="s">
+      <c r="AD2" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="AD2" s="39" t="s">
+      <c r="AE2" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AK2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AL2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AM2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AN2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AO2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AO2" s="6" t="s">
+      <c r="AP2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AP2" s="6" t="s">
+      <c r="AQ2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="AQ2" s="40" t="s">
+      <c r="AR2" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="AR2" s="40" t="s">
+      <c r="AS2" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="AS2" s="41" t="s">
+      <c r="AT2" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="AT2" s="7" t="s">
+      <c r="AU2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AU2" s="6" t="s">
+      <c r="AV2" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="AV2" s="6" t="s">
+      <c r="AW2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AW2" s="6" t="s">
+      <c r="AX2" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AY2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AY2" s="6" t="s">
+      <c r="AZ2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AZ2" s="6" t="s">
+      <c r="BA2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="BA2" s="6" t="s">
+      <c r="BB2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="BB2" s="6" t="s">
+      <c r="BC2" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="BC2" s="6" t="s">
+      <c r="BD2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="BD2" s="6" t="s">
+      <c r="BE2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="BE2" s="6" t="s">
+      <c r="BF2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="BF2" s="6" t="s">
+      <c r="BG2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="BG2" s="6" t="s">
+      <c r="BH2" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="BH2" s="6" t="s">
+      <c r="BI2" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="BI2" s="7" t="s">
+      <c r="BJ2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="BJ2" s="7" t="s">
+      <c r="BK2" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="BK2" s="13" t="s">
+      <c r="BL2" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="BL2" s="13" t="s">
+      <c r="BM2" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="BM2" s="13" t="s">
+      <c r="BN2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="BN2" s="13" t="s">
+      <c r="BO2" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="BO2" s="13" t="s">
+      <c r="BP2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="BP2" s="13" t="s">
+      <c r="BQ2" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="BQ2" s="15" t="s">
+      <c r="BR2" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="BR2" s="15" t="s">
+      <c r="BS2" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="BS2" s="15" t="s">
+      <c r="BT2" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="BT2" s="15" t="s">
+      <c r="BU2" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="BU2" s="15" t="s">
+      <c r="BV2" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="BV2" s="15" t="s">
+      <c r="BW2" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="BW2" s="15" t="s">
+      <c r="BX2" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="BX2" s="15" t="s">
+      <c r="BY2" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="BY2" s="15" t="s">
+      <c r="BZ2" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="BZ2" s="15" t="s">
+      <c r="CA2" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="CA2" s="15" t="s">
+      <c r="CB2" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="CB2" s="15" t="s">
+      <c r="CC2" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="CC2" s="15" t="s">
+      <c r="CD2" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="CD2" s="15" t="s">
+      <c r="CE2" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="CE2" s="15" t="s">
+      <c r="CF2" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="CF2" s="15" t="s">
+      <c r="CG2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="CG2" s="15" t="s">
+      <c r="CH2" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="CH2" s="15" t="s">
+      <c r="CI2" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="CI2" s="6" t="s">
+      <c r="CJ2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="CJ2" s="7" t="s">
+      <c r="CK2" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:88" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="73" t="s">
+    <row r="3" spans="1:89" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="D3" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="E3" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="37"/>
+      <c r="G3" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="H3" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="37" t="s">
+      <c r="I3" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="J3" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="J3" s="37">
+      <c r="K3" s="37">
         <v>2</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="L3" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="37" t="s">
+      <c r="M3" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="37">
+      <c r="N3" s="37">
         <v>9052125456</v>
       </c>
-      <c r="N3" s="37" t="s">
+      <c r="O3" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="37" t="s">
+      <c r="P3" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="37" t="s">
+      <c r="Q3" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="37" t="s">
+      <c r="R3" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="37" t="s">
+      <c r="S3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="S3" s="42" t="s">
+      <c r="T3" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="T3" s="37" t="s">
+      <c r="U3" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="U3" s="37">
+      <c r="V3" s="37">
         <v>9052125251</v>
       </c>
-      <c r="V3" s="37" t="s">
+      <c r="W3" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="W3" s="37" t="s">
+      <c r="X3" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="X3" s="37" t="s">
+      <c r="Y3" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="Y3" s="43" t="s">
+      <c r="Z3" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="Z3" s="37" t="s">
+      <c r="AA3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="37" t="s">
+      <c r="AB3" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="AB3" s="43" t="s">
+      <c r="AC3" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="AC3" s="44" t="s">
+      <c r="AD3" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="AD3" s="37" t="s">
+      <c r="AE3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="AE3" s="37"/>
       <c r="AF3" s="37"/>
       <c r="AG3" s="37"/>
       <c r="AH3" s="37"/>
@@ -3106,34 +3120,34 @@
       <c r="AQ3" s="37"/>
       <c r="AR3" s="37"/>
       <c r="AS3" s="37"/>
-      <c r="AT3" s="37" t="s">
+      <c r="AT3" s="37"/>
+      <c r="AU3" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="AU3" s="37">
+      <c r="AV3" s="37">
         <v>1</v>
       </c>
-      <c r="AV3" s="37"/>
       <c r="AW3" s="37"/>
-      <c r="AX3" s="37" t="s">
+      <c r="AX3" s="37"/>
+      <c r="AY3" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="AY3" s="37">
+      <c r="AZ3" s="37">
         <v>2</v>
       </c>
-      <c r="AZ3" s="37"/>
       <c r="BA3" s="37"/>
       <c r="BB3" s="37"/>
       <c r="BC3" s="37"/>
-      <c r="BD3" s="37" t="s">
-        <v>0</v>
-      </c>
+      <c r="BD3" s="37"/>
       <c r="BE3" s="37" t="s">
         <v>0</v>
       </c>
       <c r="BF3" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG3" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="BG3" s="37"/>
       <c r="BH3" s="37"/>
       <c r="BI3" s="37"/>
       <c r="BJ3" s="37"/>
@@ -3161,109 +3175,112 @@
       <c r="CF3" s="37"/>
       <c r="CG3" s="37"/>
       <c r="CH3" s="37"/>
-      <c r="CI3" s="37" t="s">
+      <c r="CI3" s="37"/>
+      <c r="CJ3" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="CJ3" s="45">
+      <c r="CK3" s="45">
         <v>1234567890</v>
       </c>
     </row>
-    <row r="4" spans="1:88" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="73"/>
-      <c r="C4" s="48" t="s">
+    <row r="4" spans="1:89" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="73"/>
+      <c r="D4" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="E4" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="26"/>
+      <c r="G4" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="H4" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="I4" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="J4" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="J4" s="26">
+      <c r="K4" s="26">
         <v>4</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="L4" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="26" t="s">
+      <c r="M4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="26">
+      <c r="N4" s="26">
         <v>9052125456</v>
       </c>
-      <c r="N4" s="26" t="s">
+      <c r="O4" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="26" t="s">
+      <c r="P4" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="26" t="s">
+      <c r="Q4" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="26" t="s">
+      <c r="R4" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="R4" s="26" t="s">
+      <c r="S4" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="T4" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="T4" s="26" t="s">
+      <c r="U4" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="U4" s="26">
+      <c r="V4" s="26">
         <v>9012367890</v>
       </c>
-      <c r="V4" s="26" t="s">
+      <c r="W4" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="W4" s="26" t="s">
+      <c r="X4" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="X4" s="26" t="s">
+      <c r="Y4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="Y4" s="27" t="s">
+      <c r="Z4" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="Z4" s="26" t="s">
+      <c r="AA4" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="26" t="s">
+      <c r="AB4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="AB4" s="28" t="s">
+      <c r="AC4" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="AC4" s="29" t="s">
+      <c r="AD4" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="AD4" s="26" t="s">
+      <c r="AE4" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="AE4" s="30" t="s">
+      <c r="AF4" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="AF4" s="30" t="s">
+      <c r="AG4" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="AG4" s="30"/>
-      <c r="AH4" s="26"/>
-      <c r="AI4" s="30"/>
+      <c r="AH4" s="30"/>
+      <c r="AI4" s="26"/>
       <c r="AJ4" s="30"/>
       <c r="AK4" s="30"/>
-      <c r="AL4" s="26"/>
+      <c r="AL4" s="30"/>
       <c r="AM4" s="26"/>
       <c r="AN4" s="26"/>
       <c r="AO4" s="26"/>
@@ -3271,34 +3288,34 @@
       <c r="AQ4" s="26"/>
       <c r="AR4" s="26"/>
       <c r="AS4" s="26"/>
-      <c r="AT4" s="26" t="s">
+      <c r="AT4" s="26"/>
+      <c r="AU4" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="AU4" s="26">
+      <c r="AV4" s="26">
         <v>1</v>
       </c>
-      <c r="AV4" s="26"/>
       <c r="AW4" s="26"/>
-      <c r="AX4" s="26" t="s">
+      <c r="AX4" s="26"/>
+      <c r="AY4" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="AY4" s="26">
+      <c r="AZ4" s="26">
         <v>4</v>
       </c>
-      <c r="AZ4" s="26"/>
       <c r="BA4" s="26"/>
       <c r="BB4" s="26"/>
       <c r="BC4" s="26"/>
-      <c r="BD4" s="26" t="s">
-        <v>0</v>
-      </c>
+      <c r="BD4" s="26"/>
       <c r="BE4" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="BF4" s="30"/>
+      <c r="BF4" s="26" t="s">
+        <v>0</v>
+      </c>
       <c r="BG4" s="30"/>
       <c r="BH4" s="30"/>
-      <c r="BI4" s="26"/>
+      <c r="BI4" s="30"/>
       <c r="BJ4" s="26"/>
       <c r="BK4" s="26"/>
       <c r="BL4" s="26"/>
@@ -3325,93 +3342,96 @@
       <c r="CG4" s="26"/>
       <c r="CH4" s="26"/>
       <c r="CI4" s="26"/>
-      <c r="CJ4" s="31"/>
-    </row>
-    <row r="5" spans="1:88" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="73"/>
-      <c r="C5" s="48" t="s">
+      <c r="CJ4" s="26"/>
+      <c r="CK4" s="31"/>
+    </row>
+    <row r="5" spans="1:89" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="73"/>
+      <c r="D5" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="E5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="26"/>
+      <c r="G5" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="H5" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="I5" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="J5" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="J5" s="26">
+      <c r="K5" s="26">
         <v>20</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="L5" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="26" t="s">
+      <c r="M5" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="26">
+      <c r="N5" s="26">
         <v>9052125456</v>
       </c>
-      <c r="N5" s="26" t="s">
+      <c r="O5" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="26" t="s">
+      <c r="P5" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="P5" s="26" t="s">
+      <c r="Q5" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="Q5" s="26" t="s">
+      <c r="R5" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="R5" s="26" t="s">
+      <c r="S5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="S5" s="24" t="s">
+      <c r="T5" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="T5" s="26" t="s">
+      <c r="U5" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="U5" s="26">
+      <c r="V5" s="26">
         <v>9012367890</v>
       </c>
-      <c r="V5" s="26" t="s">
+      <c r="W5" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="W5" s="26" t="s">
+      <c r="X5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="X5" s="26" t="s">
+      <c r="Y5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="Y5" s="27" t="s">
+      <c r="Z5" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="Z5" s="26" t="s">
+      <c r="AA5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="AA5" s="26" t="s">
+      <c r="AB5" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="AB5" s="28" t="s">
+      <c r="AC5" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="AC5" s="29" t="s">
+      <c r="AD5" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="AD5" s="26" t="s">
+      <c r="AE5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="AE5" s="26"/>
       <c r="AF5" s="26"/>
       <c r="AG5" s="26"/>
       <c r="AH5" s="26"/>
@@ -3426,54 +3446,54 @@
       <c r="AQ5" s="26"/>
       <c r="AR5" s="26"/>
       <c r="AS5" s="26"/>
-      <c r="AT5" s="26" t="s">
+      <c r="AT5" s="26"/>
+      <c r="AU5" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="AU5" s="26">
+      <c r="AV5" s="26">
         <v>1</v>
       </c>
-      <c r="AV5" s="26" t="s">
+      <c r="AW5" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="AW5" s="26">
+      <c r="AX5" s="26">
         <v>50000</v>
       </c>
-      <c r="AX5" s="26" t="s">
+      <c r="AY5" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="AY5" s="26">
+      <c r="AZ5" s="26">
         <v>20</v>
       </c>
-      <c r="AZ5" s="26">
+      <c r="BA5" s="26">
         <v>30</v>
-      </c>
-      <c r="BA5" s="26">
-        <v>12</v>
       </c>
       <c r="BB5" s="26">
         <v>12</v>
       </c>
-      <c r="BC5" s="26" t="s">
+      <c r="BC5" s="26">
+        <v>12</v>
+      </c>
+      <c r="BD5" s="26" t="s">
         <v>34</v>
-      </c>
-      <c r="BD5" s="26" t="s">
-        <v>0</v>
       </c>
       <c r="BE5" s="26" t="s">
         <v>0</v>
       </c>
       <c r="BF5" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG5" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="BG5" s="26"/>
       <c r="BH5" s="26"/>
-      <c r="BI5" s="26">
+      <c r="BI5" s="26"/>
+      <c r="BJ5" s="26">
         <v>5</v>
       </c>
-      <c r="BJ5" s="26" t="s">
+      <c r="BK5" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="BK5" s="26"/>
       <c r="BL5" s="26"/>
       <c r="BM5" s="26"/>
       <c r="BN5" s="26"/>
@@ -3498,344 +3518,348 @@
       <c r="CG5" s="26"/>
       <c r="CH5" s="26"/>
       <c r="CI5" s="26"/>
-      <c r="CJ5" s="31"/>
-    </row>
-    <row r="6" spans="1:88" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="73"/>
-      <c r="C6" s="48" t="s">
+      <c r="CJ5" s="26"/>
+      <c r="CK5" s="31"/>
+    </row>
+    <row r="6" spans="1:89" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="73"/>
+      <c r="D6" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="E6" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="24"/>
+      <c r="G6" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="H6" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="I6" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="J6" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="J6" s="26">
+      <c r="K6" s="26">
         <v>15</v>
       </c>
-      <c r="K6" s="26" t="s">
+      <c r="L6" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="26" t="s">
+      <c r="M6" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="26">
+      <c r="N6" s="26">
         <v>9052125456</v>
       </c>
-      <c r="N6" s="26" t="s">
+      <c r="O6" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="26" t="s">
+      <c r="P6" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="P6" s="26" t="s">
+      <c r="Q6" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="Q6" s="26" t="s">
+      <c r="R6" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="R6" s="26" t="s">
+      <c r="S6" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="S6" s="26" t="s">
+      <c r="T6" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="T6" s="24" t="s">
+      <c r="U6" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="U6" s="26">
+      <c r="V6" s="26">
         <v>9012367890</v>
       </c>
-      <c r="V6" s="26" t="s">
+      <c r="W6" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="W6" s="26" t="s">
+      <c r="X6" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="X6" s="26" t="s">
+      <c r="Y6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="Y6" s="26" t="s">
+      <c r="Z6" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="Z6" s="27" t="s">
+      <c r="AA6" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="AA6" s="26" t="s">
+      <c r="AB6" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="AB6" s="26" t="s">
+      <c r="AC6" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="AC6" s="29" t="s">
+      <c r="AD6" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="AD6" s="26" t="s">
+      <c r="AE6" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="AE6" s="26"/>
-      <c r="AF6" s="30"/>
+      <c r="AF6" s="26"/>
       <c r="AG6" s="30"/>
       <c r="AH6" s="30"/>
-      <c r="AI6" s="26"/>
-      <c r="AJ6" s="30"/>
+      <c r="AI6" s="30"/>
+      <c r="AJ6" s="26"/>
       <c r="AK6" s="30"/>
       <c r="AL6" s="30"/>
-      <c r="AM6" s="26"/>
+      <c r="AM6" s="30"/>
       <c r="AN6" s="26"/>
       <c r="AO6" s="26"/>
       <c r="AP6" s="26"/>
       <c r="AQ6" s="26"/>
       <c r="AR6" s="26"/>
       <c r="AS6" s="26"/>
-      <c r="AT6" s="26" t="s">
+      <c r="AT6" s="26"/>
+      <c r="AU6" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="AU6" s="26">
+      <c r="AV6" s="26">
         <v>1</v>
       </c>
-      <c r="AV6" s="26"/>
       <c r="AW6" s="26"/>
-      <c r="AX6" s="26" t="s">
+      <c r="AX6" s="26"/>
+      <c r="AY6" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="AY6" s="26">
+      <c r="AZ6" s="26">
         <v>15</v>
       </c>
-      <c r="AZ6" s="26">
+      <c r="BA6" s="26">
         <v>30</v>
-      </c>
-      <c r="BA6" s="26">
-        <v>12</v>
       </c>
       <c r="BB6" s="26">
         <v>12</v>
       </c>
-      <c r="BC6" s="26" t="s">
+      <c r="BC6" s="26">
+        <v>12</v>
+      </c>
+      <c r="BD6" s="26" t="s">
         <v>34</v>
-      </c>
-      <c r="BD6" s="26" t="s">
-        <v>0</v>
       </c>
       <c r="BE6" s="26" t="s">
         <v>0</v>
       </c>
       <c r="BF6" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG6" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="BG6" s="30"/>
       <c r="BH6" s="30"/>
       <c r="BI6" s="30"/>
-      <c r="BJ6" s="26"/>
+      <c r="BJ6" s="30"/>
       <c r="BK6" s="26"/>
       <c r="BL6" s="26"/>
       <c r="BM6" s="26"/>
       <c r="BN6" s="26"/>
       <c r="BO6" s="26"/>
       <c r="BP6" s="26"/>
-      <c r="BQ6" s="26" t="s">
+      <c r="BQ6" s="26"/>
+      <c r="BR6" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="BR6" s="26" t="b">
+      <c r="BS6" s="26" t="b">
         <v>1</v>
       </c>
-      <c r="BS6" s="26" t="s">
+      <c r="BT6" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="BT6" s="26" t="s">
+      <c r="BU6" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="BU6" s="26">
+      <c r="BV6" s="26">
         <v>1</v>
       </c>
-      <c r="BV6" s="26">
+      <c r="BW6" s="26">
         <v>1888</v>
       </c>
-      <c r="BW6" s="26">
+      <c r="BX6" s="26">
         <v>1</v>
       </c>
-      <c r="BX6" s="26" t="s">
+      <c r="BY6" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="BY6" s="26">
+      <c r="BZ6" s="26">
         <v>1</v>
       </c>
-      <c r="BZ6" s="26">
+      <c r="CA6" s="26">
         <v>680</v>
       </c>
-      <c r="CA6" s="26" t="s">
+      <c r="CB6" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="CB6" s="26">
+      <c r="CC6" s="26">
         <v>6.1</v>
       </c>
-      <c r="CC6" s="26">
+      <c r="CD6" s="26">
         <v>1</v>
       </c>
-      <c r="CD6" s="26" t="s">
+      <c r="CE6" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="CE6" s="26" t="s">
+      <c r="CF6" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="CF6" s="26" t="s">
+      <c r="CG6" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="CG6" s="26" t="s">
+      <c r="CH6" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="CH6" s="26">
+      <c r="CI6" s="26">
         <v>9015551234</v>
       </c>
-      <c r="CI6" s="26"/>
-      <c r="CJ6" s="31"/>
-    </row>
-    <row r="7" spans="1:88" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="73"/>
-      <c r="C7" s="49" t="s">
+      <c r="CJ6" s="26"/>
+      <c r="CK6" s="31"/>
+    </row>
+    <row r="7" spans="1:89" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="73"/>
+      <c r="D7" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="E7" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="E7" s="26"/>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="26"/>
+      <c r="G7" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="H7" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="H7" s="32" t="s">
+      <c r="I7" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="J7" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="32">
+      <c r="K7" s="32">
         <v>15</v>
       </c>
-      <c r="K7" s="32" t="s">
+      <c r="L7" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="L7" s="32" t="s">
+      <c r="M7" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="32">
+      <c r="N7" s="32">
         <v>9052125456</v>
       </c>
-      <c r="N7" s="26" t="s">
+      <c r="O7" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="32" t="s">
+      <c r="P7" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="P7" s="32" t="s">
+      <c r="Q7" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="Q7" s="32" t="s">
+      <c r="R7" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="R7" s="32" t="s">
+      <c r="S7" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="S7" s="25" t="s">
+      <c r="T7" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="T7" s="32" t="s">
+      <c r="U7" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="U7" s="32">
+      <c r="V7" s="32">
         <v>9052125251</v>
       </c>
-      <c r="V7" s="32" t="s">
+      <c r="W7" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="W7" s="32" t="s">
+      <c r="X7" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="X7" s="32" t="s">
+      <c r="Y7" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="Y7" s="33" t="s">
+      <c r="Z7" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="Z7" s="32" t="s">
+      <c r="AA7" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="AA7" s="32" t="s">
+      <c r="AB7" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="AB7" s="34" t="s">
+      <c r="AC7" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="AC7" s="35" t="s">
+      <c r="AD7" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="AD7" s="32" t="s">
+      <c r="AE7" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="AE7" s="32" t="s">
+      <c r="AF7" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="AF7" s="32"/>
       <c r="AG7" s="32"/>
-      <c r="AH7" s="32">
+      <c r="AH7" s="32"/>
+      <c r="AI7" s="32">
         <v>8004633339</v>
       </c>
-      <c r="AI7" s="10" t="s">
+      <c r="AJ7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AJ7" s="10" t="s">
+      <c r="AK7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK7" s="10">
+      <c r="AL7" s="10">
         <v>9012633035</v>
       </c>
-      <c r="AL7" s="26" t="s">
+      <c r="AM7" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="AM7" s="26" t="s">
+      <c r="AN7" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="AN7" s="26" t="s">
+      <c r="AO7" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="AO7" s="26" t="s">
+      <c r="AP7" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="AP7" s="32" t="s">
+      <c r="AQ7" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="AQ7" s="32"/>
       <c r="AR7" s="32"/>
       <c r="AS7" s="32"/>
-      <c r="AT7" s="32" t="s">
+      <c r="AT7" s="32"/>
+      <c r="AU7" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="AU7" s="32">
+      <c r="AV7" s="32">
         <v>1</v>
       </c>
-      <c r="AV7" s="32"/>
       <c r="AW7" s="32"/>
-      <c r="AX7" s="32" t="s">
+      <c r="AX7" s="32"/>
+      <c r="AY7" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="AY7" s="32">
+      <c r="AZ7" s="32">
         <v>15</v>
-      </c>
-      <c r="AZ7" s="32">
-        <v>25</v>
       </c>
       <c r="BA7" s="32">
         <v>25</v>
@@ -3843,16 +3867,18 @@
       <c r="BB7" s="32">
         <v>25</v>
       </c>
-      <c r="BC7" s="32" t="s">
+      <c r="BC7" s="32">
+        <v>25</v>
+      </c>
+      <c r="BD7" s="32" t="s">
         <v>34</v>
-      </c>
-      <c r="BD7" s="32" t="s">
-        <v>0</v>
       </c>
       <c r="BE7" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="BF7" s="32"/>
+      <c r="BF7" s="32" t="s">
+        <v>0</v>
+      </c>
       <c r="BG7" s="32"/>
       <c r="BH7" s="32"/>
       <c r="BI7" s="32"/>
@@ -3882,143 +3908,144 @@
       <c r="CG7" s="32"/>
       <c r="CH7" s="32"/>
       <c r="CI7" s="32"/>
-      <c r="CJ7" s="36"/>
-    </row>
-    <row r="8" spans="1:88" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="73"/>
-      <c r="C8" s="49" t="s">
+      <c r="CJ7" s="32"/>
+      <c r="CK7" s="36"/>
+    </row>
+    <row r="8" spans="1:89" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="73"/>
+      <c r="D8" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="E8" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="26"/>
+      <c r="G8" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="H8" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="I8" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="J8" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="J8" s="32">
+      <c r="K8" s="32">
         <v>15</v>
       </c>
-      <c r="K8" s="32" t="s">
+      <c r="L8" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="32" t="s">
+      <c r="M8" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="32">
+      <c r="N8" s="32">
         <v>9052125456</v>
       </c>
-      <c r="N8" s="26" t="s">
+      <c r="O8" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O8" s="32" t="s">
+      <c r="P8" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="P8" s="32" t="s">
+      <c r="Q8" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="Q8" s="32" t="s">
+      <c r="R8" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="R8" s="32" t="s">
+      <c r="S8" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="S8" s="25" t="s">
+      <c r="T8" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="T8" s="32" t="s">
+      <c r="U8" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="U8" s="32">
+      <c r="V8" s="32">
         <v>9052125251</v>
       </c>
-      <c r="V8" s="32" t="s">
+      <c r="W8" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="W8" s="32" t="s">
+      <c r="X8" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="X8" s="32" t="s">
+      <c r="Y8" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="Y8" s="33" t="s">
+      <c r="Z8" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="Z8" s="32" t="s">
+      <c r="AA8" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="AA8" s="32" t="s">
+      <c r="AB8" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="AB8" s="34" t="s">
+      <c r="AC8" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="AC8" s="35" t="s">
+      <c r="AD8" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="AD8" s="32" t="s">
+      <c r="AE8" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="AE8" s="32" t="s">
+      <c r="AF8" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="AF8" s="32"/>
       <c r="AG8" s="32"/>
-      <c r="AH8" s="32">
+      <c r="AH8" s="32"/>
+      <c r="AI8" s="32">
         <v>8004633339</v>
       </c>
-      <c r="AI8" s="10" t="s">
+      <c r="AJ8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AJ8" s="10" t="s">
+      <c r="AK8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK8" s="10">
+      <c r="AL8" s="10">
         <v>9012633035</v>
       </c>
-      <c r="AL8" s="32" t="s">
+      <c r="AM8" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="AM8" s="26" t="s">
+      <c r="AN8" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="AN8" s="26" t="s">
+      <c r="AO8" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="AO8" s="26" t="s">
+      <c r="AP8" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="AP8" s="32" t="s">
+      <c r="AQ8" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="AQ8" s="32"/>
       <c r="AR8" s="32"/>
       <c r="AS8" s="32"/>
-      <c r="AT8" s="32" t="s">
+      <c r="AT8" s="32"/>
+      <c r="AU8" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="AU8" s="32">
+      <c r="AV8" s="32">
         <v>1</v>
       </c>
-      <c r="AV8" s="32"/>
       <c r="AW8" s="32"/>
-      <c r="AX8" s="32" t="s">
+      <c r="AX8" s="32"/>
+      <c r="AY8" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="AY8" s="32">
+      <c r="AZ8" s="32">
         <v>15</v>
-      </c>
-      <c r="AZ8" s="32">
-        <v>25</v>
       </c>
       <c r="BA8" s="32">
         <v>25</v>
@@ -4026,16 +4053,18 @@
       <c r="BB8" s="32">
         <v>25</v>
       </c>
-      <c r="BC8" s="32" t="s">
+      <c r="BC8" s="32">
+        <v>25</v>
+      </c>
+      <c r="BD8" s="32" t="s">
         <v>34</v>
-      </c>
-      <c r="BD8" s="32" t="s">
-        <v>0</v>
       </c>
       <c r="BE8" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="BF8" s="32"/>
+      <c r="BF8" s="32" t="s">
+        <v>0</v>
+      </c>
       <c r="BG8" s="32"/>
       <c r="BH8" s="32"/>
       <c r="BI8" s="32"/>
@@ -4065,148 +4094,151 @@
       <c r="CG8" s="32"/>
       <c r="CH8" s="32"/>
       <c r="CI8" s="32"/>
-      <c r="CJ8" s="36"/>
-    </row>
-    <row r="9" spans="1:88" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="73"/>
-      <c r="C9" s="49" t="s">
+      <c r="CJ8" s="32"/>
+      <c r="CK8" s="36"/>
+    </row>
+    <row r="9" spans="1:89" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="73"/>
+      <c r="D9" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="E9" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="26"/>
+      <c r="G9" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="H9" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="I9" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="I9" s="32" t="s">
+      <c r="J9" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="J9" s="32">
+      <c r="K9" s="32">
         <v>20</v>
       </c>
-      <c r="K9" s="32" t="s">
+      <c r="L9" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="L9" s="32" t="s">
+      <c r="M9" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M9" s="32">
+      <c r="N9" s="32">
         <v>9052125456</v>
       </c>
-      <c r="N9" s="26" t="s">
+      <c r="O9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="32" t="s">
+      <c r="P9" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="P9" s="32" t="s">
+      <c r="Q9" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="Q9" s="32" t="s">
+      <c r="R9" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="R9" s="32" t="s">
+      <c r="S9" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="S9" s="25" t="s">
+      <c r="T9" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="T9" s="32" t="s">
+      <c r="U9" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="U9" s="32">
+      <c r="V9" s="32">
         <v>9012367890</v>
       </c>
-      <c r="V9" s="32" t="s">
+      <c r="W9" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="W9" s="32" t="s">
+      <c r="X9" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="X9" s="32" t="s">
+      <c r="Y9" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="Y9" s="33" t="s">
+      <c r="Z9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="Z9" s="32" t="s">
+      <c r="AA9" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="AA9" s="32" t="s">
+      <c r="AB9" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" s="34" t="s">
+      <c r="AC9" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="AC9" s="35" t="s">
+      <c r="AD9" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="AD9" s="32" t="s">
+      <c r="AE9" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="AE9" s="32" t="s">
+      <c r="AF9" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="AF9" s="32"/>
-      <c r="AG9" s="32" t="s">
+      <c r="AG9" s="32"/>
+      <c r="AH9" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="AH9" s="32"/>
-      <c r="AI9" s="10"/>
+      <c r="AI9" s="32"/>
       <c r="AJ9" s="10"/>
       <c r="AK9" s="10"/>
-      <c r="AL9" s="32"/>
-      <c r="AM9" s="26"/>
+      <c r="AL9" s="10"/>
+      <c r="AM9" s="32"/>
       <c r="AN9" s="26"/>
       <c r="AO9" s="26"/>
-      <c r="AP9" s="32"/>
+      <c r="AP9" s="26"/>
       <c r="AQ9" s="32"/>
       <c r="AR9" s="32"/>
       <c r="AS9" s="32"/>
-      <c r="AT9" s="32" t="s">
+      <c r="AT9" s="32"/>
+      <c r="AU9" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="AU9" s="32">
+      <c r="AV9" s="32">
         <v>1</v>
       </c>
-      <c r="AV9" s="32" t="s">
+      <c r="AW9" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="AW9" s="32">
+      <c r="AX9" s="32">
         <v>50000</v>
       </c>
-      <c r="AX9" s="32" t="s">
+      <c r="AY9" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="AY9" s="32">
+      <c r="AZ9" s="32">
         <v>20</v>
       </c>
-      <c r="AZ9" s="32">
+      <c r="BA9" s="32">
         <v>30</v>
-      </c>
-      <c r="BA9" s="32">
-        <v>12</v>
       </c>
       <c r="BB9" s="32">
         <v>12</v>
       </c>
-      <c r="BC9" s="32" t="s">
+      <c r="BC9" s="32">
+        <v>12</v>
+      </c>
+      <c r="BD9" s="32" t="s">
         <v>34</v>
-      </c>
-      <c r="BD9" s="32" t="s">
-        <v>0</v>
       </c>
       <c r="BE9" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="BF9" s="32"/>
+      <c r="BF9" s="32" t="s">
+        <v>0</v>
+      </c>
       <c r="BG9" s="32"/>
       <c r="BH9" s="32"/>
       <c r="BI9" s="32"/>
@@ -4236,139 +4268,142 @@
       <c r="CG9" s="32"/>
       <c r="CH9" s="32"/>
       <c r="CI9" s="32"/>
-      <c r="CJ9" s="36"/>
-    </row>
-    <row r="10" spans="1:88" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="73"/>
-      <c r="C10" s="49" t="s">
+      <c r="CJ9" s="32"/>
+      <c r="CK9" s="36"/>
+    </row>
+    <row r="10" spans="1:89" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="73"/>
+      <c r="D10" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="E10" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="26"/>
+      <c r="G10" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="H10" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="H10" s="32" t="s">
+      <c r="I10" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="I10" s="32" t="s">
+      <c r="J10" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="J10" s="32">
+      <c r="K10" s="32">
         <v>15</v>
       </c>
-      <c r="K10" s="32" t="s">
+      <c r="L10" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="32" t="s">
+      <c r="M10" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M10" s="32">
+      <c r="N10" s="32">
         <v>9052125456</v>
       </c>
-      <c r="N10" s="26" t="s">
+      <c r="O10" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="32" t="s">
+      <c r="P10" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="P10" s="32" t="s">
+      <c r="Q10" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="Q10" s="32" t="s">
+      <c r="R10" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="R10" s="32" t="s">
+      <c r="S10" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="25" t="s">
+      <c r="T10" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="T10" s="32" t="s">
+      <c r="U10" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="U10" s="32">
+      <c r="V10" s="32">
         <v>9012367890</v>
       </c>
-      <c r="V10" s="32" t="s">
+      <c r="W10" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="W10" s="32" t="s">
+      <c r="X10" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="X10" s="32" t="s">
+      <c r="Y10" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="Y10" s="33" t="s">
+      <c r="Z10" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="Z10" s="32" t="s">
+      <c r="AA10" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="AA10" s="32" t="s">
+      <c r="AB10" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="AB10" s="34" t="s">
+      <c r="AC10" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="AC10" s="35" t="s">
+      <c r="AD10" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="AD10" s="32" t="s">
+      <c r="AE10" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="AE10" s="32"/>
       <c r="AF10" s="32"/>
       <c r="AG10" s="32"/>
       <c r="AH10" s="32"/>
-      <c r="AI10" s="10"/>
+      <c r="AI10" s="32"/>
       <c r="AJ10" s="10"/>
       <c r="AK10" s="10"/>
-      <c r="AL10" s="32"/>
-      <c r="AM10" s="26"/>
+      <c r="AL10" s="10"/>
+      <c r="AM10" s="32"/>
       <c r="AN10" s="26"/>
       <c r="AO10" s="26"/>
-      <c r="AP10" s="32"/>
+      <c r="AP10" s="26"/>
       <c r="AQ10" s="32"/>
       <c r="AR10" s="32"/>
       <c r="AS10" s="32"/>
-      <c r="AT10" s="32" t="s">
+      <c r="AT10" s="32"/>
+      <c r="AU10" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="AU10" s="32">
+      <c r="AV10" s="32">
         <v>1</v>
       </c>
-      <c r="AV10" s="32"/>
       <c r="AW10" s="32"/>
-      <c r="AX10" s="32" t="s">
+      <c r="AX10" s="32"/>
+      <c r="AY10" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="AY10" s="32">
+      <c r="AZ10" s="32">
         <v>15</v>
       </c>
-      <c r="AZ10" s="32"/>
       <c r="BA10" s="32"/>
       <c r="BB10" s="32"/>
       <c r="BC10" s="32"/>
-      <c r="BD10" s="32" t="s">
-        <v>0</v>
-      </c>
+      <c r="BD10" s="32"/>
       <c r="BE10" s="32" t="s">
         <v>0</v>
       </c>
       <c r="BF10" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG10" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="BG10" s="32"/>
-      <c r="BH10" s="32" t="s">
+      <c r="BH10" s="32"/>
+      <c r="BI10" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="BI10" s="32"/>
       <c r="BJ10" s="32"/>
       <c r="BK10" s="32"/>
       <c r="BL10" s="32"/>
@@ -4395,141 +4430,144 @@
       <c r="CG10" s="32"/>
       <c r="CH10" s="32"/>
       <c r="CI10" s="32"/>
-      <c r="CJ10" s="36"/>
-    </row>
-    <row r="11" spans="1:88" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="73"/>
-      <c r="C11" s="49" t="s">
+      <c r="CJ10" s="32"/>
+      <c r="CK10" s="36"/>
+    </row>
+    <row r="11" spans="1:89" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="73"/>
+      <c r="D11" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="E11" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="E11" s="26"/>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="26"/>
+      <c r="G11" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="H11" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="I11" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="32" t="s">
+      <c r="J11" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="J11" s="32">
+      <c r="K11" s="32">
         <v>15</v>
       </c>
-      <c r="K11" s="32" t="s">
+      <c r="L11" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="L11" s="32" t="s">
+      <c r="M11" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="32">
+      <c r="N11" s="32">
         <v>9052125456</v>
       </c>
-      <c r="N11" s="26" t="s">
+      <c r="O11" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="32" t="s">
+      <c r="P11" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="P11" s="32" t="s">
+      <c r="Q11" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="Q11" s="32" t="s">
+      <c r="R11" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="R11" s="32" t="s">
+      <c r="S11" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="S11" s="25" t="s">
+      <c r="T11" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="T11" s="32" t="s">
+      <c r="U11" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="U11" s="32">
+      <c r="V11" s="32">
         <v>9012367890</v>
       </c>
-      <c r="V11" s="32" t="s">
+      <c r="W11" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="W11" s="32" t="s">
+      <c r="X11" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="X11" s="32" t="s">
+      <c r="Y11" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="Y11" s="33" t="s">
+      <c r="Z11" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="Z11" s="32" t="s">
+      <c r="AA11" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="AA11" s="32" t="s">
+      <c r="AB11" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="AB11" s="34" t="s">
+      <c r="AC11" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="AC11" s="35" t="s">
+      <c r="AD11" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="AD11" s="32" t="s">
+      <c r="AE11" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="AE11" s="32"/>
       <c r="AF11" s="32"/>
       <c r="AG11" s="32"/>
       <c r="AH11" s="32"/>
-      <c r="AI11" s="10"/>
+      <c r="AI11" s="32"/>
       <c r="AJ11" s="10"/>
       <c r="AK11" s="10"/>
-      <c r="AL11" s="32"/>
-      <c r="AM11" s="26"/>
+      <c r="AL11" s="10"/>
+      <c r="AM11" s="32"/>
       <c r="AN11" s="26"/>
       <c r="AO11" s="26"/>
-      <c r="AP11" s="32"/>
+      <c r="AP11" s="26"/>
       <c r="AQ11" s="32"/>
       <c r="AR11" s="32"/>
       <c r="AS11" s="32"/>
-      <c r="AT11" s="32" t="s">
+      <c r="AT11" s="32"/>
+      <c r="AU11" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="AU11" s="32">
+      <c r="AV11" s="32">
         <v>1</v>
       </c>
-      <c r="AV11" s="32"/>
       <c r="AW11" s="32"/>
-      <c r="AX11" s="32" t="s">
+      <c r="AX11" s="32"/>
+      <c r="AY11" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="AY11" s="32">
+      <c r="AZ11" s="32">
         <v>15</v>
       </c>
-      <c r="AZ11" s="32"/>
       <c r="BA11" s="32"/>
       <c r="BB11" s="32"/>
       <c r="BC11" s="32"/>
-      <c r="BD11" s="32" t="s">
-        <v>0</v>
-      </c>
+      <c r="BD11" s="32"/>
       <c r="BE11" s="32" t="s">
         <v>0</v>
       </c>
       <c r="BF11" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG11" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="BG11" s="32" t="s">
+      <c r="BH11" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="BH11" s="32" t="s">
+      <c r="BI11" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="BI11" s="32"/>
       <c r="BJ11" s="32"/>
       <c r="BK11" s="32"/>
       <c r="BL11" s="32"/>
@@ -4556,143 +4594,144 @@
       <c r="CG11" s="32"/>
       <c r="CH11" s="32"/>
       <c r="CI11" s="32"/>
-      <c r="CJ11" s="36"/>
-    </row>
-    <row r="12" spans="1:88" s="2" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="74"/>
-      <c r="C12" s="54" t="s">
+      <c r="CJ11" s="32"/>
+      <c r="CK11" s="36"/>
+    </row>
+    <row r="12" spans="1:89" s="2" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="78" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="74"/>
+      <c r="D12" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="55" t="s">
+      <c r="E12" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56" t="s">
+      <c r="F12" s="56"/>
+      <c r="G12" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="56" t="s">
+      <c r="H12" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="H12" s="56" t="s">
+      <c r="I12" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="I12" s="56" t="s">
+      <c r="J12" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="J12" s="56">
+      <c r="K12" s="56">
         <v>15</v>
       </c>
-      <c r="K12" s="56" t="s">
+      <c r="L12" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="L12" s="56" t="s">
+      <c r="M12" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="56">
+      <c r="N12" s="56">
         <v>9052125456</v>
       </c>
-      <c r="N12" s="56" t="s">
+      <c r="O12" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="O12" s="56" t="s">
+      <c r="P12" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="P12" s="56" t="s">
+      <c r="Q12" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="Q12" s="56" t="s">
+      <c r="R12" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="R12" s="56" t="s">
+      <c r="S12" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="S12" s="55" t="s">
+      <c r="T12" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="T12" s="56" t="s">
+      <c r="U12" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="U12" s="56">
+      <c r="V12" s="56">
         <v>9052125251</v>
       </c>
-      <c r="V12" s="56" t="s">
+      <c r="W12" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="W12" s="56" t="s">
+      <c r="X12" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="X12" s="56" t="s">
+      <c r="Y12" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="Y12" s="57" t="s">
+      <c r="Z12" s="57" t="s">
         <v>120</v>
       </c>
-      <c r="Z12" s="56" t="s">
+      <c r="AA12" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="AA12" s="56" t="s">
+      <c r="AB12" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="AB12" s="58" t="s">
+      <c r="AC12" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="AC12" s="59" t="s">
+      <c r="AD12" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="AD12" s="56" t="s">
+      <c r="AE12" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="AE12" s="60" t="s">
+      <c r="AF12" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="AF12" s="60"/>
       <c r="AG12" s="60"/>
-      <c r="AH12" s="56">
+      <c r="AH12" s="60"/>
+      <c r="AI12" s="56">
         <v>8004633339</v>
       </c>
-      <c r="AI12" s="61" t="s">
+      <c r="AJ12" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="AJ12" s="61" t="s">
+      <c r="AK12" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="AK12" s="46">
+      <c r="AL12" s="46">
         <v>9012633035</v>
       </c>
-      <c r="AL12" s="56" t="s">
+      <c r="AM12" s="56" t="s">
         <v>119</v>
       </c>
-      <c r="AM12" s="56" t="s">
+      <c r="AN12" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="AN12" s="56" t="s">
+      <c r="AO12" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="AO12" s="56" t="s">
+      <c r="AP12" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="AP12" s="56" t="s">
+      <c r="AQ12" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="AQ12" s="56"/>
       <c r="AR12" s="56"/>
       <c r="AS12" s="56"/>
-      <c r="AT12" s="56" t="s">
+      <c r="AT12" s="56"/>
+      <c r="AU12" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="AU12" s="56">
+      <c r="AV12" s="56">
         <v>1</v>
       </c>
-      <c r="AV12" s="56"/>
       <c r="AW12" s="56"/>
-      <c r="AX12" s="56" t="s">
+      <c r="AX12" s="56"/>
+      <c r="AY12" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="AY12" s="56">
+      <c r="AZ12" s="56">
         <v>15</v>
-      </c>
-      <c r="AZ12" s="56">
-        <v>25</v>
       </c>
       <c r="BA12" s="56">
         <v>25</v>
@@ -4700,19 +4739,21 @@
       <c r="BB12" s="56">
         <v>25</v>
       </c>
-      <c r="BC12" s="56" t="s">
+      <c r="BC12" s="56">
+        <v>25</v>
+      </c>
+      <c r="BD12" s="56" t="s">
         <v>34</v>
-      </c>
-      <c r="BD12" s="56" t="s">
-        <v>0</v>
       </c>
       <c r="BE12" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="BF12" s="60"/>
-      <c r="BG12" s="61"/>
+      <c r="BF12" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG12" s="60"/>
       <c r="BH12" s="61"/>
-      <c r="BI12" s="56"/>
+      <c r="BI12" s="61"/>
       <c r="BJ12" s="56"/>
       <c r="BK12" s="56"/>
       <c r="BL12" s="56"/>
@@ -4739,102 +4780,105 @@
       <c r="CG12" s="56"/>
       <c r="CH12" s="56"/>
       <c r="CI12" s="56"/>
-      <c r="CJ12" s="62"/>
-    </row>
-    <row r="13" spans="1:88" s="2" customFormat="1" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="75" t="s">
+      <c r="CJ12" s="56"/>
+      <c r="CK12" s="62"/>
+    </row>
+    <row r="13" spans="1:89" s="2" customFormat="1" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="78" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="75" t="s">
         <v>181</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="D13" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="64" t="s">
+      <c r="E13" s="64" t="s">
         <v>171</v>
       </c>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65" t="s">
+      <c r="F13" s="65"/>
+      <c r="G13" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="G13" s="65" t="s">
+      <c r="H13" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="H13" s="65" t="s">
+      <c r="I13" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="I13" s="65" t="s">
+      <c r="J13" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="J13" s="65">
+      <c r="K13" s="65">
         <v>15</v>
       </c>
-      <c r="K13" s="65" t="s">
+      <c r="L13" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="L13" s="65" t="s">
+      <c r="M13" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="M13" s="65">
+      <c r="N13" s="65">
         <v>9052125456</v>
       </c>
-      <c r="N13" s="65" t="s">
+      <c r="O13" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="O13" s="65" t="s">
+      <c r="P13" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="P13" s="65" t="s">
+      <c r="Q13" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="Q13" s="65" t="s">
+      <c r="R13" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="R13" s="65" t="s">
+      <c r="S13" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="S13" s="64" t="s">
+      <c r="T13" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="T13" s="65" t="s">
+      <c r="U13" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="U13" s="65">
+      <c r="V13" s="65">
         <v>9012367890</v>
       </c>
-      <c r="V13" s="65" t="s">
+      <c r="W13" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="W13" s="65" t="s">
+      <c r="X13" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="X13" s="65" t="s">
+      <c r="Y13" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="Y13" s="66" t="s">
+      <c r="Z13" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="Z13" s="65" t="s">
+      <c r="AA13" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="AA13" s="65" t="s">
+      <c r="AB13" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="AB13" s="67" t="s">
+      <c r="AC13" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="AC13" s="68" t="s">
+      <c r="AD13" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="AD13" s="65" t="s">
+      <c r="AE13" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="AE13" s="69"/>
       <c r="AF13" s="69"/>
       <c r="AG13" s="69"/>
-      <c r="AH13" s="65"/>
-      <c r="AI13" s="69"/>
+      <c r="AH13" s="69"/>
+      <c r="AI13" s="65"/>
       <c r="AJ13" s="69"/>
       <c r="AK13" s="69"/>
-      <c r="AL13" s="65"/>
+      <c r="AL13" s="69"/>
       <c r="AM13" s="65"/>
       <c r="AN13" s="65"/>
       <c r="AO13" s="65"/>
@@ -4842,44 +4886,44 @@
       <c r="AQ13" s="65"/>
       <c r="AR13" s="65"/>
       <c r="AS13" s="65"/>
-      <c r="AT13" s="65" t="s">
+      <c r="AT13" s="65"/>
+      <c r="AU13" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="AU13" s="65">
+      <c r="AV13" s="65">
         <v>1</v>
       </c>
-      <c r="AV13" s="65"/>
       <c r="AW13" s="65"/>
-      <c r="AX13" s="65" t="s">
+      <c r="AX13" s="65"/>
+      <c r="AY13" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="AY13" s="65">
+      <c r="AZ13" s="65">
         <v>15</v>
       </c>
-      <c r="AZ13" s="65">
+      <c r="BA13" s="65">
         <v>30</v>
-      </c>
-      <c r="BA13" s="65">
-        <v>12</v>
       </c>
       <c r="BB13" s="65">
         <v>12</v>
       </c>
-      <c r="BC13" s="65" t="s">
+      <c r="BC13" s="65">
+        <v>12</v>
+      </c>
+      <c r="BD13" s="65" t="s">
         <v>34</v>
-      </c>
-      <c r="BD13" s="65" t="s">
-        <v>0</v>
       </c>
       <c r="BE13" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="BF13" s="69" t="s">
+      <c r="BF13" s="65" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG13" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="BG13" s="70"/>
       <c r="BH13" s="70"/>
-      <c r="BI13" s="65"/>
+      <c r="BI13" s="70"/>
       <c r="BJ13" s="65"/>
       <c r="BK13" s="65"/>
       <c r="BL13" s="65"/>
@@ -4887,148 +4931,151 @@
       <c r="BN13" s="65"/>
       <c r="BO13" s="65"/>
       <c r="BP13" s="65"/>
-      <c r="BQ13" s="65" t="s">
+      <c r="BQ13" s="65"/>
+      <c r="BR13" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="BR13" s="65" t="b">
+      <c r="BS13" s="65" t="b">
         <v>1</v>
       </c>
-      <c r="BS13" s="65" t="s">
+      <c r="BT13" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="BT13" s="65" t="s">
+      <c r="BU13" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="BU13" s="65">
+      <c r="BV13" s="65">
         <v>1</v>
       </c>
-      <c r="BV13" s="65">
+      <c r="BW13" s="65">
         <v>1888</v>
       </c>
-      <c r="BW13" s="65">
+      <c r="BX13" s="65">
         <v>1</v>
       </c>
-      <c r="BX13" s="65" t="s">
+      <c r="BY13" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="BY13" s="65">
+      <c r="BZ13" s="65">
         <v>1</v>
       </c>
-      <c r="BZ13" s="65">
+      <c r="CA13" s="65">
         <v>680</v>
       </c>
-      <c r="CA13" s="65" t="s">
+      <c r="CB13" s="65" t="s">
         <v>133</v>
       </c>
-      <c r="CB13" s="65">
+      <c r="CC13" s="65">
         <v>6.1</v>
       </c>
-      <c r="CC13" s="65">
+      <c r="CD13" s="65">
         <v>1</v>
       </c>
-      <c r="CD13" s="65" t="s">
+      <c r="CE13" s="65" t="s">
         <v>134</v>
       </c>
-      <c r="CE13" s="65" t="s">
+      <c r="CF13" s="65" t="s">
         <v>136</v>
       </c>
-      <c r="CF13" s="65" t="s">
+      <c r="CG13" s="65" t="s">
         <v>137</v>
       </c>
-      <c r="CG13" s="65" t="s">
+      <c r="CH13" s="65" t="s">
         <v>139</v>
       </c>
-      <c r="CH13" s="65">
+      <c r="CI13" s="65">
         <v>9015551234</v>
       </c>
-      <c r="CI13" s="65"/>
-      <c r="CJ13" s="71"/>
-    </row>
-    <row r="14" spans="1:88" s="2" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="76"/>
-      <c r="C14" s="72" t="s">
+      <c r="CJ13" s="65"/>
+      <c r="CK13" s="71"/>
+    </row>
+    <row r="14" spans="1:89" s="2" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="78" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" s="76"/>
+      <c r="D14" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="E14" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38" t="s">
+      <c r="F14" s="38"/>
+      <c r="G14" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="H14" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="38" t="s">
+      <c r="I14" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="I14" s="38" t="s">
+      <c r="J14" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="J14" s="38">
+      <c r="K14" s="38">
         <v>15</v>
       </c>
-      <c r="K14" s="38" t="s">
+      <c r="L14" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="L14" s="38" t="s">
+      <c r="M14" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="38">
+      <c r="N14" s="38">
         <v>9052125456</v>
       </c>
-      <c r="N14" s="38" t="s">
+      <c r="O14" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O14" s="38" t="s">
+      <c r="P14" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="P14" s="38" t="s">
+      <c r="Q14" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="Q14" s="38" t="s">
+      <c r="R14" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="R14" s="38" t="s">
+      <c r="S14" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="S14" s="50" t="s">
+      <c r="T14" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="T14" s="38" t="s">
+      <c r="U14" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="U14" s="38">
+      <c r="V14" s="38">
         <v>9012367890</v>
       </c>
-      <c r="V14" s="38" t="s">
+      <c r="W14" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="W14" s="38" t="s">
+      <c r="X14" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="X14" s="38" t="s">
+      <c r="Y14" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="Y14" s="51" t="s">
+      <c r="Z14" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="Z14" s="38" t="s">
+      <c r="AA14" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="AA14" s="38" t="s">
+      <c r="AB14" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="AB14" s="52" t="s">
+      <c r="AC14" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="AC14" s="11" t="s">
+      <c r="AD14" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AD14" s="38" t="s">
+      <c r="AE14" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="AE14" s="38"/>
       <c r="AF14" s="38"/>
       <c r="AG14" s="38"/>
       <c r="AH14" s="38"/>
@@ -5043,26 +5090,24 @@
       <c r="AQ14" s="38"/>
       <c r="AR14" s="38"/>
       <c r="AS14" s="38"/>
-      <c r="AT14" s="38" t="s">
+      <c r="AT14" s="38"/>
+      <c r="AU14" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="AU14" s="38">
+      <c r="AV14" s="38">
         <v>2</v>
       </c>
-      <c r="AV14" s="38" t="s">
+      <c r="AW14" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="AW14" s="38">
+      <c r="AX14" s="38">
         <v>12500</v>
       </c>
-      <c r="AX14" s="38" t="s">
+      <c r="AY14" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="AY14" s="38">
+      <c r="AZ14" s="38">
         <v>42</v>
-      </c>
-      <c r="AZ14" s="38">
-        <v>25</v>
       </c>
       <c r="BA14" s="38">
         <v>25</v>
@@ -5070,16 +5115,18 @@
       <c r="BB14" s="38">
         <v>25</v>
       </c>
-      <c r="BC14" s="38" t="s">
+      <c r="BC14" s="38">
+        <v>25</v>
+      </c>
+      <c r="BD14" s="38" t="s">
         <v>34</v>
-      </c>
-      <c r="BD14" s="38" t="s">
-        <v>0</v>
       </c>
       <c r="BE14" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="BF14" s="38"/>
+      <c r="BF14" s="38" t="s">
+        <v>0</v>
+      </c>
       <c r="BG14" s="38"/>
       <c r="BH14" s="38"/>
       <c r="BI14" s="38"/>
@@ -5109,13 +5156,14 @@
       <c r="CG14" s="38"/>
       <c r="CH14" s="38"/>
       <c r="CI14" s="38"/>
-      <c r="CJ14" s="53"/>
-    </row>
-    <row r="15" spans="1:88" s="2" customFormat="1" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="CJ14" s="38"/>
+      <c r="CK14" s="53"/>
+    </row>
+    <row r="15" spans="1:89" s="2" customFormat="1" ht="12.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C15" s="1"/>
       <c r="Y15" s="3"/>
     </row>
-    <row r="16" spans="1:88" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:89" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
       <c r="Y16" s="3"/>
     </row>
@@ -8140,8 +8188,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B3:B12"/>
-    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C3:C12"/>
+    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>